<commit_message>
Updated example build files and updated components workbook
Added the 'build from scratch' files into their own subfolder and added a second template file.

Added a level interpolation example to the components workbook.
</commit_message>
<xml_diff>
--- a/Simulator Component Workbook.xlsx
+++ b/Simulator Component Workbook.xlsx
@@ -8,20 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sawtoothsoftware-my.sharepoint.com/personal/kenneth_sawtoothsoftware_com/Documents/GitHub/ExcelSimulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{FAFCD64C-CC42-4406-8A6D-BBD73641E7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C001CC66-AA8F-471E-AC0D-85549702329E}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{FAFCD64C-CC42-4406-8A6D-BBD73641E7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABAF6542-49E4-4527-BCD0-E02F07C66C75}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Base Simulator" sheetId="1" r:id="rId1"/>
+    <sheet name="Simulator with Interpolation" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Design">Sheet1!$D$22:$H$31</definedName>
-    <definedName name="ProductInclude">Sheet1!$D$16:$H$16</definedName>
-    <definedName name="RespondentInclude">Sheet1!$M$17:$M$26</definedName>
-    <definedName name="rng">Sheet1!#REF!</definedName>
-    <definedName name="Utilities">Sheet1!$N$17:$W$26</definedName>
-    <definedName name="Weights">Sheet1!$X$17:$X$26</definedName>
+    <definedName name="Design">'Base Simulator'!$D$22:$H$31</definedName>
+    <definedName name="InterpolationDesign">'Simulator with Interpolation'!$D$22:$H$31</definedName>
+    <definedName name="InterpolationProductInclude">'Simulator with Interpolation'!$D$16:$H$16</definedName>
+    <definedName name="InterpolationRespondentInclude">'Simulator with Interpolation'!$M$17:$M$26</definedName>
+    <definedName name="InterpolationUtilities">'Simulator with Interpolation'!$N$17:$W$26</definedName>
+    <definedName name="InterpolationWeights">'Simulator with Interpolation'!$X$17:$X$26</definedName>
+    <definedName name="ProductInclude">'Base Simulator'!$D$16:$H$16</definedName>
+    <definedName name="RespondentInclude">'Base Simulator'!$M$17:$M$26</definedName>
+    <definedName name="rng">'Base Simulator'!#REF!</definedName>
+    <definedName name="Utilities">'Base Simulator'!$N$17:$W$26</definedName>
+    <definedName name="Weights">'Base Simulator'!$X$17:$X$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -221,8 +227,75 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4F5A4627-0C83-4224-BC8F-AFDCFB896F88}</author>
+    <author>tc={B406D49B-C027-4127-AF08-F371261FF2A8}</author>
+    <author>tc={9C244862-CCD1-4CA1-9BED-EE00516B9F07}</author>
+    <author>tc={E62E0BAD-4200-41F8-97D1-AFF2E8FCBF42}</author>
+    <author>tc={177DC505-0F5F-48B1-93A8-670E28B6D286}</author>
+    <author>tc={82401466-D6FD-4257-9768-435617439E0D}</author>
+  </authors>
+  <commentList>
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{4F5A4627-0C83-4224-BC8F-AFDCFB896F88}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    One value below the range and one above just make it so the formula can be dragged cleanly across all cells, only the highlighted rows matter.</t>
+      </text>
+    </comment>
+    <comment ref="P5" authorId="1" shapeId="0" xr:uid="{B406D49B-C027-4127-AF08-F371261FF2A8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is where the actual interpolation values are computed
+Reply:
+    The main linear interpolation formula is (cell-RangeMin)/(RangeMax-RangeMin)
+The rest of the formula is just a yes/no logic to get the right math for the right range. 
+E.g. If you're between 1 and 2. If you're at 1.1, you should be 0.9 weighted at 1, and 0.1 weighted at 2.</t>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="2" shapeId="0" xr:uid="{9C244862-CCD1-4CA1-9BED-EE00516B9F07}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These values are changed to be validated as a 'decimal' value between $1 and $3</t>
+      </text>
+    </comment>
+    <comment ref="K12" authorId="3" shapeId="0" xr:uid="{E62E0BAD-4200-41F8-97D1-AFF2E8FCBF42}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These labels are no longer used</t>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="4" shapeId="0" xr:uid="{177DC505-0F5F-48B1-93A8-670E28B6D286}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These values are no longer a lookup of the simulator page, they just reflect the values directly</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="5" shapeId="0" xr:uid="{82401466-D6FD-4257-9768-435617439E0D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These values are no longer a calculation from the values above, but refer directly to the interpolation calculations.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="36">
   <si>
     <t>Red</t>
   </si>
@@ -325,15 +398,45 @@
   <si>
     <t>Total Utility 5</t>
   </si>
+  <si>
+    <t>Interpolation Calculation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cells modified from base are in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and commented</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,8 +478,16 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +497,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,7 +778,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -691,13 +808,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -729,6 +870,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Kenneth Fairchild" id="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" userId="Kenneth Fairchild" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -992,13 +1139,39 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="O4" dT="2020-04-28T17:45:43.30" personId="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" id="{4F5A4627-0C83-4224-BC8F-AFDCFB896F88}">
+    <text>One value below the range and one above just make it so the formula can be dragged cleanly across all cells, only the highlighted rows matter.</text>
+  </threadedComment>
+  <threadedComment ref="P5" dT="2020-04-28T17:44:44.86" personId="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" id="{B406D49B-C027-4127-AF08-F371261FF2A8}">
+    <text>This is where the actual interpolation values are computed</text>
+  </threadedComment>
+  <threadedComment ref="P5" dT="2020-04-28T17:51:47.13" personId="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" id="{C25B421F-DD26-4433-934C-C0FC49553B94}" parentId="{B406D49B-C027-4127-AF08-F371261FF2A8}">
+    <text>The main linear interpolation formula is (cell-RangeMin)/(RangeMax-RangeMin)
+The rest of the formula is just a yes/no logic to get the right math for the right range. 
+E.g. If you're between 1 and 2. If you're at 1.1, you should be 0.9 weighted at 1, and 0.1 weighted at 2.</text>
+  </threadedComment>
+  <threadedComment ref="D6" dT="2020-04-28T17:42:40.48" personId="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" id="{9C244862-CCD1-4CA1-9BED-EE00516B9F07}">
+    <text>These values are changed to be validated as a 'decimal' value between $1 and $3</text>
+  </threadedComment>
+  <threadedComment ref="K12" dT="2020-04-28T17:55:50.84" personId="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" id="{E62E0BAD-4200-41F8-97D1-AFF2E8FCBF42}">
+    <text>These labels are no longer used</text>
+  </threadedComment>
+  <threadedComment ref="G19" dT="2020-04-28T17:43:39.92" personId="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" id="{177DC505-0F5F-48B1-93A8-670E28B6D286}">
+    <text>These values are no longer a lookup of the simulator page, they just reflect the values directly</text>
+  </threadedComment>
+  <threadedComment ref="D28" dT="2020-04-28T17:44:28.39" personId="{B43F80DE-5BC4-42F9-BF02-F4A5A51F091C}" id="{82401466-D6FD-4257-9768-435617439E0D}">
+    <text>These values are no longer a calculation from the values above, but refer directly to the interpolation calculations.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AJ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2802,14 +2975,14 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D3:H3">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:G4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$K$6:$K$8</formula1>
     </dataValidation>
@@ -2830,4 +3003,1319 @@
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518676DD-3237-42B0-8755-C398811B1202}">
+  <dimension ref="A1:X35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2"/>
+      <c r="O2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="29">
+        <f>AND(D$19&gt;=$O4,D$19&lt;$O5)*((D$19-$O4)/($O5-$O4))+
+  AND(D$19&gt;=$O5,D$19&lt;$O6)*(1-(D$19-$O5)/($O6-$O5))</f>
+        <v>0.99</v>
+      </c>
+      <c r="Q5" s="29">
+        <f t="shared" ref="Q5:S5" si="0">AND(E$19&gt;=$O4,E$19&lt;$O5)*((E$19-$O4)/($O5-$O4))+
+  AND(E$19&gt;=$O5,E$19&lt;$O6)*(1-(E$19-$O5)/($O6-$O5))</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="31">
+        <v>1.01</v>
+      </c>
+      <c r="E6" s="31">
+        <v>2.25</v>
+      </c>
+      <c r="F6" s="31">
+        <v>2.75</v>
+      </c>
+      <c r="G6" s="31">
+        <v>2</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <v>2</v>
+      </c>
+      <c r="P6" s="29">
+        <f t="shared" ref="P6:P7" si="1">AND(D$19&gt;=$O5,D$19&lt;$O6)*((D$19-$O5)/($O6-$O5))+
+  AND(D$19&gt;=$O6,D$19&lt;$O7)*(1-(D$19-$O6)/($O7-$O6))</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="Q6" s="29">
+        <f t="shared" ref="Q6:Q7" si="2">AND(E$19&gt;=$O5,E$19&lt;$O6)*((E$19-$O5)/($O6-$O5))+
+  AND(E$19&gt;=$O6,E$19&lt;$O7)*(1-(E$19-$O6)/($O7-$O6))</f>
+        <v>0.75</v>
+      </c>
+      <c r="R6" s="29">
+        <f t="shared" ref="R6:R7" si="3">AND(F$19&gt;=$O5,F$19&lt;$O6)*((F$19-$O5)/($O6-$O5))+
+  AND(F$19&gt;=$O6,F$19&lt;$O7)*(1-(F$19-$O6)/($O7-$O6))</f>
+        <v>0.25</v>
+      </c>
+      <c r="S6" s="32">
+        <f t="shared" ref="S6:S7" si="4">AND(G$19&gt;=$O5,G$19&lt;$O6)*((G$19-$O5)/($O6-$O5))+
+  AND(G$19&gt;=$O6,G$19&lt;$O7)*(1-(G$19-$O6)/($O7-$O6))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>2</v>
+      </c>
+      <c r="O7" s="3">
+        <v>3</v>
+      </c>
+      <c r="P7" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="29">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="R7" s="29">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="S7" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
+      <c r="C8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="23">
+        <f>K30</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
+        <f>L30</f>
+        <v>1.6373937025027971E-2</v>
+      </c>
+      <c r="F8" s="23">
+        <f>M30</f>
+        <v>7.4471290537957546E-3</v>
+      </c>
+      <c r="G8" s="23">
+        <f>N30</f>
+        <v>2.4698528118794773E-2</v>
+      </c>
+      <c r="H8" s="24">
+        <f>O30</f>
+        <v>0.95148040580238169</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="5">
+        <v>3</v>
+      </c>
+      <c r="O8" s="7">
+        <v>4</v>
+      </c>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J9" s="3"/>
+      <c r="K9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J10" s="3"/>
+      <c r="K10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J11" s="3"/>
+      <c r="K11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J12" s="3"/>
+      <c r="K12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+      <c r="K13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="7"/>
+      <c r="K14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <f>1*(D3="Include")</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f>1*(E3="Include")</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <f>1*(F3="Include")</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <f>1*(G3="Include")</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <f>1*(H3="Include")</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X16" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" ref="D17:G19" si="5">VLOOKUP(D4,$K$6:$L$14,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="4">
+        <v>-3.6234906809517637</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1.0017380409445025</v>
+      </c>
+      <c r="P17" s="4">
+        <v>2.6217526400072613</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>-2.1595092491668759</v>
+      </c>
+      <c r="R17" s="4">
+        <v>-0.81361518618904993</v>
+      </c>
+      <c r="S17" s="4">
+        <v>2.9731244353559259</v>
+      </c>
+      <c r="T17" s="4">
+        <v>3.3232777112663836</v>
+      </c>
+      <c r="U17" s="4">
+        <v>-0.57623882460399356</v>
+      </c>
+      <c r="V17" s="4">
+        <v>-2.74703888666239</v>
+      </c>
+      <c r="W17" s="5">
+        <v>-0.6637837060640166</v>
+      </c>
+      <c r="X17" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4">
+        <v>2</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
+      <c r="N18" s="4">
+        <v>-0.80942405210077695</v>
+      </c>
+      <c r="O18" s="4">
+        <v>-0.34354688798646382</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1.1529709400872408</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>-4.5389422159422264</v>
+      </c>
+      <c r="R18" s="4">
+        <v>1.8983101366976927</v>
+      </c>
+      <c r="S18" s="4">
+        <v>2.6406320792445337</v>
+      </c>
+      <c r="T18" s="4">
+        <v>1.6182630544367367</v>
+      </c>
+      <c r="U18" s="4">
+        <v>-0.40938601768766247</v>
+      </c>
+      <c r="V18" s="4">
+        <v>-1.2088770367490742</v>
+      </c>
+      <c r="W18" s="5">
+        <v>1.545042404194124</v>
+      </c>
+      <c r="X18" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="30">
+        <f>D6</f>
+        <v>1.01</v>
+      </c>
+      <c r="E19" s="30">
+        <f t="shared" ref="E19:G19" si="6">E6</f>
+        <v>2.25</v>
+      </c>
+      <c r="F19" s="30">
+        <f t="shared" si="6"/>
+        <v>2.75</v>
+      </c>
+      <c r="G19" s="30">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4">
+        <v>3</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1</v>
+      </c>
+      <c r="N19" s="4">
+        <v>-2.7382290409865537</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1.0592317126917781</v>
+      </c>
+      <c r="P19" s="4">
+        <v>1.6789973282947757</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>-0.73895587578903932</v>
+      </c>
+      <c r="R19" s="4">
+        <v>-9.7894924837435671E-2</v>
+      </c>
+      <c r="S19" s="4">
+        <v>0.83685080062647499</v>
+      </c>
+      <c r="T19" s="4">
+        <v>2.8317967758110196</v>
+      </c>
+      <c r="U19" s="4">
+        <v>-0.85675621312899386</v>
+      </c>
+      <c r="V19" s="4">
+        <v>-1.9750405626820255</v>
+      </c>
+      <c r="W19" s="5">
+        <v>-1.6269166279206462</v>
+      </c>
+      <c r="X19" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="5"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4">
+        <v>4</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4">
+        <v>-1.9956515376533084</v>
+      </c>
+      <c r="O20" s="4">
+        <v>-0.56261921400905801</v>
+      </c>
+      <c r="P20" s="4">
+        <v>2.5582707516623664</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>-1.2301553514877654</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0.40314139672182003</v>
+      </c>
+      <c r="S20" s="4">
+        <v>0.82701395476594541</v>
+      </c>
+      <c r="T20" s="4">
+        <v>0.66185991160424229</v>
+      </c>
+      <c r="U20" s="4">
+        <v>0.61852681170604562</v>
+      </c>
+      <c r="V20" s="4">
+        <v>-1.2803867233102879</v>
+      </c>
+      <c r="W20" s="5">
+        <v>-1.0034852923994482</v>
+      </c>
+      <c r="X20" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4">
+        <v>3</v>
+      </c>
+      <c r="G21" s="4">
+        <v>4</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4">
+        <v>5</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
+      <c r="N21" s="4">
+        <v>-1.4604352378315344</v>
+      </c>
+      <c r="O21" s="4">
+        <v>-0.23222168346732808</v>
+      </c>
+      <c r="P21" s="4">
+        <v>1.6926569212988625</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>-1.8158593763926805</v>
+      </c>
+      <c r="R21" s="4">
+        <v>-0.35355392593739565</v>
+      </c>
+      <c r="S21" s="4">
+        <v>2.1694133023300761</v>
+      </c>
+      <c r="T21" s="4">
+        <v>2.7572259968761799</v>
+      </c>
+      <c r="U21" s="4">
+        <v>-0.31874165768128737</v>
+      </c>
+      <c r="V21" s="4">
+        <v>-2.4384843391948925</v>
+      </c>
+      <c r="W21" s="5">
+        <v>1.8722463714826922</v>
+      </c>
+      <c r="X21" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <f>1*(VLOOKUP($B22,$B$17:$G$19,D$21+2,0)=$C22)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" ref="E22:G30" si="7">1*(VLOOKUP($B22,$B$17:$G$19,E$21+2,0)=$C22)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4">
+        <v>6</v>
+      </c>
+      <c r="M22" s="4">
+        <v>1</v>
+      </c>
+      <c r="N22" s="4">
+        <v>-2.2838712058546169</v>
+      </c>
+      <c r="O22" s="4">
+        <v>5.2384805288376857E-2</v>
+      </c>
+      <c r="P22" s="4">
+        <v>2.23148640056624</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>-0.72781888837503406</v>
+      </c>
+      <c r="R22" s="4">
+        <v>-0.17690277077403671</v>
+      </c>
+      <c r="S22" s="4">
+        <v>0.90472165914907077</v>
+      </c>
+      <c r="T22" s="4">
+        <v>0.68610473572202735</v>
+      </c>
+      <c r="U22" s="4">
+        <v>0.621646938817773</v>
+      </c>
+      <c r="V22" s="4">
+        <v>-1.3077516745398003</v>
+      </c>
+      <c r="W22" s="5">
+        <v>1.5132259848662661</v>
+      </c>
+      <c r="X22" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" ref="D23:D30" si="8">1*(VLOOKUP($B23,$B$17:$G$19,D$21+2,0)=$C23)</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4">
+        <v>7</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
+      <c r="N23" s="4">
+        <v>-1.459969830214795</v>
+      </c>
+      <c r="O23" s="4">
+        <v>-0.35845261155442687</v>
+      </c>
+      <c r="P23" s="4">
+        <v>1.8184224417692219</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>-1.9692163349254073</v>
+      </c>
+      <c r="R23" s="4">
+        <v>-0.88731264037003044</v>
+      </c>
+      <c r="S23" s="4">
+        <v>2.8565289752954377</v>
+      </c>
+      <c r="T23" s="4">
+        <v>1.6211753250503467</v>
+      </c>
+      <c r="U23" s="4">
+        <v>-0.65915500994560983</v>
+      </c>
+      <c r="V23" s="4">
+        <v>-0.96202031510473685</v>
+      </c>
+      <c r="W23" s="5">
+        <v>1.5526881522266276</v>
+      </c>
+      <c r="X23" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4">
+        <v>8</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
+      <c r="N24" s="4">
+        <v>-1.569385126102139</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0.41314343821528876</v>
+      </c>
+      <c r="P24" s="4">
+        <v>1.1562416878868502</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>-5.1515062573876893</v>
+      </c>
+      <c r="R24" s="4">
+        <v>2.1550564397316352</v>
+      </c>
+      <c r="S24" s="4">
+        <v>2.9964498176560541</v>
+      </c>
+      <c r="T24" s="4">
+        <v>1.4293543468107419</v>
+      </c>
+      <c r="U24" s="4">
+        <v>0.20743267504439933</v>
+      </c>
+      <c r="V24" s="4">
+        <v>-1.6367870218551412</v>
+      </c>
+      <c r="W24" s="5">
+        <v>0.63175942806813135</v>
+      </c>
+      <c r="X24" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4">
+        <v>9</v>
+      </c>
+      <c r="M25" s="4">
+        <v>1</v>
+      </c>
+      <c r="N25" s="4">
+        <v>-1.033203933479321</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0.21455850098068496</v>
+      </c>
+      <c r="P25" s="4">
+        <v>0.81864543249863608</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>-4.6348456913410887</v>
+      </c>
+      <c r="R25" s="4">
+        <v>2.1952689230411471</v>
+      </c>
+      <c r="S25" s="4">
+        <v>2.4395767682999416</v>
+      </c>
+      <c r="T25" s="4">
+        <v>1.403770276338743</v>
+      </c>
+      <c r="U25" s="4">
+        <v>-9.069001789571951E-2</v>
+      </c>
+      <c r="V25" s="4">
+        <v>-1.3130802584430235</v>
+      </c>
+      <c r="W25" s="5">
+        <v>-0.5631515597305885</v>
+      </c>
+      <c r="X25" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10">
+        <v>10</v>
+      </c>
+      <c r="M26" s="10">
+        <v>1</v>
+      </c>
+      <c r="N26" s="10">
+        <v>-1.5026211672830621</v>
+      </c>
+      <c r="O26" s="10">
+        <v>-0.91920982897624404</v>
+      </c>
+      <c r="P26" s="10">
+        <v>2.4218309962593061</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>-2.0418334227990425</v>
+      </c>
+      <c r="R26" s="10">
+        <v>-0.36998533916696497</v>
+      </c>
+      <c r="S26" s="10">
+        <v>2.4118187619660074</v>
+      </c>
+      <c r="T26" s="10">
+        <v>4.8778675714801629</v>
+      </c>
+      <c r="U26" s="10">
+        <v>-1.9590992549862021</v>
+      </c>
+      <c r="V26" s="10">
+        <v>-2.9187683164939608</v>
+      </c>
+      <c r="W26" s="9">
+        <v>-0.21827878736915185</v>
+      </c>
+      <c r="X26" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="X27" s="25"/>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="29">
+        <f t="shared" ref="D28:G30" si="9">P5</f>
+        <v>0.99</v>
+      </c>
+      <c r="E28" s="29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="2"/>
+      <c r="X28" s="25"/>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2</v>
+      </c>
+      <c r="D29" s="29">
+        <f t="shared" si="9"/>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="E29" s="29">
+        <f t="shared" si="9"/>
+        <v>0.75</v>
+      </c>
+      <c r="F29" s="29">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="G29" s="29">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4">
+        <v>3</v>
+      </c>
+      <c r="D30" s="29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="29">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="F30" s="29">
+        <f t="shared" si="9"/>
+        <v>0.75</v>
+      </c>
+      <c r="G30" s="29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="10">
+        <f t="array" ref="K30:O30">MMULT(TRANSPOSE(InterpolationRespondentInclude),(EXP(MMULT(InterpolationUtilities,InterpolationDesign))*MMULT(InterpolationRespondentInclude,InterpolationProductInclude))/(MMULT(EXP(MMULT(InterpolationUtilities,InterpolationDesign)),TRANSPOSE(InterpolationProductInclude))))/SUM(InterpolationRespondentInclude)</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="10">
+        <v>1.6373937025027971E-2</v>
+      </c>
+      <c r="M30" s="10">
+        <v>7.4471290537957546E-3</v>
+      </c>
+      <c r="N30" s="10">
+        <v>2.4698528118794773E-2</v>
+      </c>
+      <c r="O30" s="9">
+        <v>0.95148040580238169</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <v>1</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J34" s="3"/>
+      <c r="K34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="10:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="10">
+        <f t="array" ref="K35:O35">MMULT(TRANSPOSE(InterpolationRespondentInclude*InterpolationWeights),(EXP(MMULT(InterpolationUtilities,InterpolationDesign))*MMULT(InterpolationRespondentInclude,InterpolationProductInclude))/(MMULT(EXP(MMULT(InterpolationUtilities,InterpolationDesign)),TRANSPOSE(InterpolationProductInclude))))/SUM(InterpolationRespondentInclude*InterpolationWeights)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="10">
+        <v>1.6373937025027971E-2</v>
+      </c>
+      <c r="M35" s="10">
+        <v>7.4471290537957546E-3</v>
+      </c>
+      <c r="N35" s="10">
+        <v>2.4698528118794773E-2</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0.95148040580238169</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:H3">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:H3" xr:uid="{8D818C83-2CB3-40EE-AF09-6EDEE6A074F8}">
+      <formula1>$K$4:$K$5</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:G6" xr:uid="{E7F3DC3A-6171-40EF-B417-D689B9670913}">
+      <formula1>1</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:G5" xr:uid="{0E977B82-3883-464B-9A40-DF45DF9E7CAD}">
+      <formula1>$K$9:$K$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:G4" xr:uid="{CBF8B516-C5B2-49BC-89EB-D0798F65C236}">
+      <formula1>$K$6:$K$8</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>